<commit_message>
feat(WriteExcel): adding path name by proyect
</commit_message>
<xml_diff>
--- a/Excels/Documentacion de empleados para cargar.xlsx
+++ b/Excels/Documentacion de empleados para cargar.xlsx
@@ -46,7 +46,7 @@
     <t>Brizuela</t>
   </si>
   <si>
-    <t>20-39004114-8</t>
+    <t>20-40729043-8</t>
   </si>
   <si>
     <t>M</t>
@@ -64,7 +64,7 @@
     <t>Aguilar</t>
   </si>
   <si>
-    <t>20-40328334-5</t>
+    <t>20-40729043-5</t>
   </si>
   <si>
     <t>Chofer</t>

</xml_diff>